<commit_message>
#4, #5, #6, #7
</commit_message>
<xml_diff>
--- a/MocaOffice20Test/Book1.xlsx
+++ b/MocaOffice20Test/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moka\Documents\Dev\CodePlex\moca\Develop\Moca.NET\DEV\Core\MocaOfficeTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moka\Documents\GitHub\mocanet\MocaOffice\MocaOffice20Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,13 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="ColA">Sheet1!$B$5:$B$9</definedName>
+    <definedName name="ColB">Sheet1!$C$5:$C$9</definedName>
+    <definedName name="ColC">Sheet1!$D$5:$D$9</definedName>
+    <definedName name="ColD">Sheet1!$E$5:$E$9</definedName>
+    <definedName name="ColE">Sheet1!$F$5:$F$9</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -407,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -505,6 +512,12 @@
         <v>43</v>
       </c>
     </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="F11" t="e">
+        <f>F5:F6</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>